<commit_message>
Changed SQL Columns reference to match new file_location.
</commit_message>
<xml_diff>
--- a/Documentation/SQL Column Translations.xlsx
+++ b/Documentation/SQL Column Translations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-13845" yWindow="1800" windowWidth="24240" windowHeight="13740" activeTab="1"/>
+    <workbookView xWindow="-13845" yWindow="1800" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="dust_event" sheetId="2" r:id="rId1"/>
@@ -407,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +434,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -448,7 +448,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +544,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -558,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>

</xml_diff>